<commit_message>
Started Orders.ToXml() and supporting methods. These are disabled in OrderWriter to use the old binary format until they are completed and tested.
</commit_message>
<xml_diff>
--- a/Documentation/Turn Files/Turn File Contents.xlsx
+++ b/Documentation/Turn Files/Turn File Contents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="81">
   <si>
     <t>ConsoleState</t>
   </si>
@@ -228,15 +228,9 @@
     <t>Proposed</t>
   </si>
   <si>
-    <t>NewTurn</t>
-  </si>
-  <si>
     <t>Universe</t>
   </si>
   <si>
-    <t>AllStars (position only)</t>
-  </si>
-  <si>
     <t>KnownMinefields</t>
   </si>
   <si>
@@ -256,6 +250,15 @@
   </si>
   <si>
     <t>+Messages (to players or self)</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>RaceData (not a RaceData object)</t>
   </si>
 </sst>
 </file>
@@ -608,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,16 +656,16 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
         <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -679,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -698,8 +701,11 @@
       <c r="H4" t="s">
         <v>6</v>
       </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
         <v>64</v>
@@ -721,8 +727,11 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L5" t="s">
         <v>63</v>
@@ -741,8 +750,11 @@
       <c r="H6" t="s">
         <v>11</v>
       </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -787,10 +799,10 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -992,10 +1004,10 @@
         <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1165,7 +1177,7 @@
         <v>51</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Standardised the way new xml documents are created in GlobalDefinitions.InitializeXmlDocument() Tidyed up of Property Tab display in component editor. Re-enabled Hull map editing in component editor.
</commit_message>
<xml_diff>
--- a/Documentation/Turn Files/Turn File Contents.xlsx
+++ b/Documentation/Turn Files/Turn File Contents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="83">
   <si>
     <t>ConsoleState</t>
   </si>
@@ -258,7 +258,13 @@
     <t>Orders</t>
   </si>
   <si>
-    <t>RaceData (not a RaceData object)</t>
+    <t>PlayerRace</t>
+  </si>
+  <si>
+    <t>BattlePlans (in PlayerData)</t>
+  </si>
+  <si>
+    <t>PlayerRelations (in PlayerData)</t>
   </si>
 </sst>
 </file>
@@ -310,11 +316,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,10 +1095,7 @@
         <v>67</v>
       </c>
       <c r="K32" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1116,10 +1120,7 @@
         <v>67</v>
       </c>
       <c r="K34" t="s">
-        <v>44</v>
-      </c>
-      <c r="L34" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1179,8 +1180,11 @@
       <c r="D39" t="s">
         <v>80</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>52</v>
+      <c r="K39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1271,6 +1275,9 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
+        <v>66</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>66</v>
       </c>
       <c r="L47" t="s">

</xml_diff>

<commit_message>
Added AllMessages (ArrayList) to the ServerState object. Messages are now created here first and appropriately copied to the intel object. Converted Intel from a Singleton to a normal instance object (as the console generates an intel file for each player). Cleared the AllMessages list at the end of the turn generation process so old messages are not repeated.
</commit_message>
<xml_diff>
--- a/Documentation/Turn Files/Turn File Contents.xlsx
+++ b/Documentation/Turn Files/Turn File Contents.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="86">
-  <si>
-    <t>ConsoleState</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="85">
   <si>
     <t>AllBattles</t>
   </si>
@@ -132,9 +129,6 @@
     <t>AlllMinefields</t>
   </si>
   <si>
-    <t>GUIstate</t>
-  </si>
-  <si>
     <t>DeletedDesigns</t>
   </si>
   <si>
@@ -274,6 +268,9 @@
   </si>
   <si>
     <t>StateFileName</t>
+  </si>
+  <si>
+    <t>AllMessages</t>
   </si>
 </sst>
 </file>
@@ -627,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,670 +643,676 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="21">
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="H26" t="s">
+        <v>84</v>
       </c>
       <c r="J26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" t="s">
         <v>53</v>
       </c>
-      <c r="D41" t="s">
-        <v>55</v>
-      </c>
       <c r="J41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fleets update which planet they are orbiting when they move. Added a warning when forcing turn generation.
</commit_message>
<xml_diff>
--- a/Documentation/Turn Files/Turn File Contents.xlsx
+++ b/Documentation/Turn Files/Turn File Contents.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="86">
   <si>
     <t>AllBattles</t>
   </si>
@@ -271,22 +271,17 @@
   </si>
   <si>
     <t>AllMessages</t>
+  </si>
+  <si>
+    <t>GameSettings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,11 +317,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -622,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,21 +629,22 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="21">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="21">
+      <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -669,19 +664,22 @@
         <v>82</v>
       </c>
       <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>76</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>81</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -694,11 +692,11 @@
       <c r="H3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -714,17 +712,14 @@
       <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>71</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -740,17 +735,17 @@
       <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>70</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -763,14 +758,14 @@
       <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -781,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -794,11 +789,11 @@
       <c r="H8" t="s">
         <v>8</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -811,14 +806,14 @@
       <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>9</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -829,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -840,7 +835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -851,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -862,7 +857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -873,7 +868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -884,7 +879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -895,7 +890,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -906,7 +901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -917,7 +912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -928,7 +923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -939,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -947,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -958,7 +953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -969,7 +964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -980,7 +975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -999,14 +994,14 @@
       <c r="H25" t="s">
         <v>15</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>15</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1022,36 +1017,36 @@
       <c r="H26" t="s">
         <v>84</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>74</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1061,14 +1056,14 @@
       <c r="E29" t="s">
         <v>37</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1078,25 +1073,25 @@
       <c r="E30" t="s">
         <v>38</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1106,22 +1101,22 @@
       <c r="E32" t="s">
         <v>65</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1131,44 +1126,44 @@
       <c r="E34" t="s">
         <v>65</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
         <v>43</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>45</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1178,132 +1173,135 @@
       <c r="E38" t="s">
         <v>63</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>49</v>
       </c>
       <c r="D39" t="s">
         <v>78</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" t="s">
         <v>78</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>51</v>
       </c>
       <c r="D40" t="s">
         <v>52</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>51</v>
       </c>
       <c r="D41" t="s">
         <v>53</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>53</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>55</v>
       </c>
       <c r="D43" t="s">
         <v>56</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>13</v>
       </c>
       <c r="D44" t="s">
         <v>57</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>58</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>16</v>
       </c>
       <c r="D46" t="s">
         <v>59</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>59</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>50</v>
       </c>
       <c r="E47" t="s">
         <v>64</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>13</v>
       </c>
       <c r="E48" t="s">
         <v>51</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>